<commit_message>
Version 1.2: Patch notes in README
</commit_message>
<xml_diff>
--- a/example/config.xlsx
+++ b/example/config.xlsx
@@ -5,19 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vrln.sharepoint.com/sites/GGD-ONDZ/PSchijf/Gezondheidsmonitor/Algemeen/Automatisering en R/0. Github/Rapportage VO en OKO/example/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanderve\OneDrive - VRLN\PSchijf\Gezondheidsmonitor\Algemeen\Automatisering en R\0. Github\report_excel_to_powerpoint\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="655" documentId="8_{61B768BC-6538-486A-86A6-2934F42D50E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1BDB9D89-9B5A-43ED-B976-D1FF78A20703}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F360C7-580E-4BC7-811C-422536A8DCD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{340DDFAE-1A83-41FC-A379-531A17E4526A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{340DDFAE-1A83-41FC-A379-531A17E4526A}"/>
   </bookViews>
   <sheets>
     <sheet name="reports" sheetId="4" r:id="rId1"/>
     <sheet name="slideconfig" sheetId="6" r:id="rId2"/>
+    <sheet name="slideconfig errors" sheetId="7" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">slideconfig!$A$1:$O$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'slideconfig errors'!$A$1:$O$21</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -472,15 +474,292 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Vermeulen, Sander</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{3A6DDAAC-DB96-4EDB-87F8-2D4C8310B620}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Deze kolom is multifunctioneel. Het gebruik van de kolom is afhankelijk van het type.
+Voor grafieken wordt deze kolom gebruikt als grafiektitel.
+Bij het type text_comparison wordt de tekst in deze kolom gebruikt om te bepalen welke vergelijking er moet worden gemaakt en welke vergelijkstext er moet worden gekozen afhankelijk van de uitkomst van de vergelijking.
+Bij het type percentage_in_text wordt deze kolom gebruikt om te bepalen waar de percentages moeten komen.
+Voor het type topN wordt deze kolom, naast de grafiektitel, ook gebruikt om te bepalen hoeveel variabelen moeten worden getoond.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{841F10B0-B2BB-43CD-8ECC-BAA3558A5298}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Voer in deze kolom het type in dat moet worden gebruikt voor deze slideregel.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{A127A259-CF63-4784-87E7-B35CF39AA8B5}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Voer hier de variabelenaam of variabelenamen in waarvoor cijfers moeten worden berekend.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{A4C88C7D-40E4-47E4-94F6-8C62D181951E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Voer hier de waarde in waarvoor cijfers moeten worden berekend. De waardes moeten overeenkomen met de opgegeven variabele naam in de kolom var. Als je meerdere variabelen hebt opgegeven in de kolom var dan geef je in deze kolom evenveel waardes op als variabelen. Scheid de waardes met een puntkomma ';'
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{D347B8B5-505A-46A1-93A7-402E51CAC44E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>In deze kolom kun je per opgegeven waarde de waardelabels aanpassen. Stel je berekent het cijfer voor value 1 en het waarde label wil je veranderen naar 'Voelt zich gelukkig' dan doe je dat zo:
+1 = Voelt zich gelukkig
+Heb je meerdere variabelen opgegeven in de kolom var (en dus ook meerdere values in de kolom value) dan moet je aangepaste labels scheiden door een puntkomma ';'. Bijvoorbeeld:
+1 = Voelt zich gelukkig; 1 = Is weerbaar
+Het script gebruikt als deze kolom leeg is de labels die in dataset zitten. Je kunt de labels dus ook zelf aanpassen in de data.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{DB53629F-11D4-49B2-B8B2-029759700076}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Geef hier een variabele naam op als je de variabele(n) in de kolom var wilt berekenen voor verschillende groepen.
+Je kunt hier meerdere variabele namen opgegeven gescheiden door een puntkomma ';'. Als je dit doet worden voor elke variabele gegroepeerde cijfers berekend op de opgegeven variabelen in de kolom var. Wil je tegelijk groeperen op twee variabelen geef dan een van de variabelen op in grouping1 en de andere in grouping 2. Doe je dit binnen een staafgrafiek dan komt grouping1 op de x-as en grouping2 in de legenda.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{24A47BC3-745F-472F-AC41-912F2B01801F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Wil je de labels van de opgegeven variabele in kolom grouping1 aanpassen geef dat dan hier op.
+Voorbeeld:
+0 = M; 1 = J
+Let op dat dit niet kan als je meerdere variabelen opgeeft in de kolom grouping1 dat dit niet werkt. Het script gebruikt als deze kolom leeg is de labels die in dataset zitten. Je kunt de labels dus ook zelf aanpassen in de data.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{EBD45C9E-A560-44E4-94FA-F2D12EC76979}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Geef hier een variabele naam op als je de variabele(n) in de kolom var wilt berekenen voor verschillende groepen.
+Je kunt hier meerdere variabele namen opgegeven gescheiden door een puntkomma ';'. Als je dit doet worden voor elke variabele gegroepeerde cijfers berekend op de opgegeven variabelen in de kolom var. Wil je tegelijk groeperen op twee variabelen geef dan een van de variabelen op in grouping1 en de andere in grouping 2. Doe je dit binnen een staafgrafiek dan komt grouping1 op de x-as en grouping2 in de legenda.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{BCBAF521-D70C-4B7A-8C12-6182D13D42F9}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Wil je de labels van de opgegeven variabele in kolom grouping1 aanpassen geef dat dan hier op.
+Voorbeeld:
+0 = M; 1 = J
+Let op dat dit niet kan als je meerdere variabelen opgeeft in de kolom grouping1 dat dit niet werkt. Het script gebruikt als deze kolom leeg is de labels die in dataset zitten. Je kunt de labels dus ook zelf aanpassen in de data.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{FC4ADE40-53A6-45B3-B68F-A8871F0BC1B9}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Geef hier de variabele naam of namen op van de dimensies waarvoor cijfers moeten worden berekend. Deze variabele moet overeenkomen met een (of meer) van de variabelen die is opgegeven in de kolom dim_vars van de rapportconfiguratie (het eerste tabblad van dit Excel bestand).
+Geef je meerdere dimensie variabelen op scheid deze dan met een puntkomma ';'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{2DE70DB4-0430-47E8-A03E-A8C4742E1601}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Vul hier de waarde in van de opgegeven time_var in de rapportconfiguratie waarvoor cijfers moeten worden berekend. Wil je voor meer dan een periode cijfersberekenen dan kun je meerdere waardes opgegeven gescheiden door een puntkomma ';'.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{37CEB835-027D-4FDB-A33A-2C83A8C26F31}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Geef hier op wat voor type weging moet worden toegepast.
+Kies je voor 'none' dan worden ongewogen cijfers berekend.
+Kies je voor 'var' dan moet je per indicator een weegfactor variabele opgeven in de kolom weight_var.
+Kies je voor 'dim' dan wordt er gewogen op dimensieniveau. Hiervoor moet je de juiste weegfactor variabele(n) opgegeven in de rapportconfiguratie (eerste tabblad van dit Excel bestand).
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{821253B3-00D0-49D0-B44F-810F98C15DDB}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Als het weight_type var is en je dus weegt op variabele niveau dan geef je hier de weegfactor voor de variabele op. Varieert de weegfactor variabele afhankelijk van bijvoorbeeld het jaar dan kun je per opgegeven jaar in de time_val kolom een weegfactor opgeven gescheiden door een puntkomma ';'
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{B3C8EC77-516D-4853-91A8-238D004968BC}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Geef hier het slidenummer op waar de content geplaatst moet worden.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{FBDED92D-F73E-4DC3-960B-85A3E379DAEF}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Geef hier de naam op van de tijdelijke aanduiding waar de content moet worden geplaatst op de opgegeven slide.
+Let op dat de opgegeven naam </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>exact</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> hetzelfde is.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{A1254F1B-23CD-424B-B31B-42CDBA4D1318}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Bij grafieken loopt de y-as standaard van 0 tot 1 (0 tot 100%). Om de hoogte van de y-as aan te passen kun je hier een waarde tussen 0 en 1 opgegeven.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{37226A97-2FAE-439E-8294-18FA874A47D4}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">De standaard richting van alle staafgrafieken is verticaal. Wil je een horizontale staafgrafiek maken vul dan bij de desbetreffende regel horizontal in.
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="118">
   <si>
     <t>Zandwijk</t>
   </si>
   <si>
-    <t>slideconfig</t>
-  </si>
-  <si>
     <t>gemeente</t>
   </si>
   <si>
@@ -619,9 +898,6 @@
     <t>text</t>
   </si>
   <si>
-    <t>reportname</t>
-  </si>
-  <si>
     <t>barchart</t>
   </si>
   <si>
@@ -649,9 +925,6 @@
     <t>grouping2_labels</t>
   </si>
   <si>
-    <t>example/data.sav</t>
-  </si>
-  <si>
     <t>example/template.pptx</t>
   </si>
   <si>
@@ -664,13 +937,7 @@
     <t>linechart</t>
   </si>
   <si>
-    <t>2024; 2020; 2016</t>
-  </si>
-  <si>
     <t>Trendgrafiek 1</t>
-  </si>
-  <si>
-    <t>weegfactor2024; weegfactor2020; weegfactor2016</t>
   </si>
   <si>
     <t>Geeft mantelzorg</t>
@@ -724,13 +991,121 @@
     <t>text_comparison</t>
   </si>
   <si>
-    <t>2024; 2020</t>
-  </si>
-  <si>
     <t>De ervaren gezondheid van jongens [grouping2 = Jongen] [is vergelijkbaar met; ligt hoger dan; ligt lager dan] meisjes [grouping2 = Meisje].</t>
   </si>
   <si>
     <t>KLAS; GENDER</t>
+  </si>
+  <si>
+    <t>De ervaren gezondheid van jongeren in klas 2 [grouping1 = Klas 2] [is vergelijkbaar met; ligt hoger dan; ligt lager dan] jongeren in klas 4 [grouping1 = Klas 4]. De ervaren gezondheid van jongens [grouping1 = Jongen] [is precies hetzelfde als; ligt super veel hoger dan; ligt super veel lager dan] meisjes [grouping1 = Meisje].</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Het percentage inwoners in uw gemeente dat een goede gezondheid ervaart in 2024 [dim_var = gemeente] is </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[vergelijkbaar met; hoger dan in; lager dan in]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Nederland [dim_var = nederland].</t>
+    </r>
+  </si>
+  <si>
+    <t>Percentage in tekst 1</t>
+  </si>
+  <si>
+    <t>Percentage in tekst 2</t>
+  </si>
+  <si>
+    <t>Percentage in tekst 3</t>
+  </si>
+  <si>
+    <t>Percentage in tekst 4</t>
+  </si>
+  <si>
+    <t>percentage_in_text</t>
+  </si>
+  <si>
+    <t>EBEGK311; PBMHK3S3</t>
+  </si>
+  <si>
+    <t>In uw gemeente ervaart EBEGK311 van de inwoners een zeer goede gezondheid.</t>
+  </si>
+  <si>
+    <t>In Nederland ervaart EBEGK311 van de inwoners een zeer goede gezondheid.</t>
+  </si>
+  <si>
+    <t>In uw gemeente ervaart EBEGK311 van de inwoners een zeer goede gezondheid en heeft PBMHK3S3 psychische klachten.</t>
+  </si>
+  <si>
+    <t>In Nederland ervaart EBEGK311 van de inwoners een zeer goede gezondheid en heeft PBMHK3S3 psychische klachten.</t>
+  </si>
+  <si>
+    <t>nederland</t>
+  </si>
+  <si>
+    <t>Staafgrafiek 5</t>
+  </si>
+  <si>
+    <t>ylimit</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>direction</t>
+  </si>
+  <si>
+    <t>horizontal</t>
+  </si>
+  <si>
+    <t>topN</t>
+  </si>
+  <si>
+    <t>topN 1</t>
+  </si>
+  <si>
+    <t>STRESS1; STRESS2; STRESS3; STRESS4; STRESS5</t>
+  </si>
+  <si>
+    <t>1; 1; 1; 1; 1</t>
+  </si>
+  <si>
+    <t>1 = Huiswerk; 1 = Thuissituatie; 1 = Werk; 1 = Ouders; 1 = Vrienden</t>
+  </si>
+  <si>
+    <t>topN 2</t>
+  </si>
+  <si>
+    <t>Top 3 bronnen van stress [3]</t>
+  </si>
+  <si>
+    <t>Rekenhulp</t>
+  </si>
+  <si>
+    <t>population_table</t>
+  </si>
+  <si>
+    <t>data/data.sav</t>
+  </si>
+  <si>
+    <t>Rekenhulp 1</t>
   </si>
   <si>
     <r>
@@ -757,103 +1132,46 @@
     </r>
   </si>
   <si>
-    <t>De ervaren gezondheid van jongeren in klas 2 [grouping1 = Klas 2] [is vergelijkbaar met; ligt hoger dan; ligt lager dan] jongeren in klas 4 [grouping1 = Klas 4]. De ervaren gezondheid van jongens [grouping1 = Jongen] [is precies hetzelfde als; ligt super veel hoger dan; ligt super veel lager dan] meisjes [grouping1 = Meisje].</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Het percentage inwoners in uw gemeente dat een goede gezondheid ervaart in 2024 [dim_var = gemeente] is </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[vergelijkbaar met; hoger dan in; lager dan in]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Nederland [dim_var = nederland].</t>
-    </r>
-  </si>
-  <si>
-    <t>Percentage in tekst 1</t>
-  </si>
-  <si>
-    <t>Percentage in tekst 2</t>
-  </si>
-  <si>
-    <t>Percentage in tekst 3</t>
-  </si>
-  <si>
-    <t>Percentage in tekst 4</t>
-  </si>
-  <si>
-    <t>percentage_in_text</t>
-  </si>
-  <si>
-    <t>EBEGK311; PBMHK3S3</t>
-  </si>
-  <si>
-    <t>In uw gemeente ervaart EBEGK311 van de inwoners een zeer goede gezondheid.</t>
-  </si>
-  <si>
-    <t>In Nederland ervaart EBEGK311 van de inwoners een zeer goede gezondheid.</t>
-  </si>
-  <si>
-    <t>In uw gemeente ervaart EBEGK311 van de inwoners een zeer goede gezondheid en heeft PBMHK3S3 psychische klachten.</t>
-  </si>
-  <si>
-    <t>In Nederland ervaart EBEGK311 van de inwoners een zeer goede gezondheid en heeft PBMHK3S3 psychische klachten.</t>
-  </si>
-  <si>
-    <t>nederland</t>
-  </si>
-  <si>
-    <t>Staafgrafiek 5</t>
-  </si>
-  <si>
-    <t>ylimit</t>
-  </si>
-  <si>
-    <t>0.3</t>
-  </si>
-  <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t>direction</t>
-  </si>
-  <si>
-    <t>horizontal</t>
-  </si>
-  <si>
-    <t>topN</t>
-  </si>
-  <si>
-    <t>topN 1</t>
-  </si>
-  <si>
-    <t>STRESS1; STRESS2; STRESS3; STRESS4; STRESS5</t>
-  </si>
-  <si>
-    <t>1; 1; 1; 1; 1</t>
-  </si>
-  <si>
-    <t>1 = Huiswerk; 1 = Thuissituatie; 1 = Werk; 1 = Ouders; 1 = Vrienden</t>
-  </si>
-  <si>
-    <t>topN 2</t>
-  </si>
-  <si>
-    <t>Top 3 bronnen van stress [3]</t>
+    <t>2024; 2022; 2020; 2016; 2012</t>
+  </si>
+  <si>
+    <t>2024; 2020</t>
+  </si>
+  <si>
+    <t>weegfactor2024; weegfactor2022; weegfactor2020; weegfactor2016; weegfactor2012</t>
+  </si>
+  <si>
+    <t>reportname</t>
+  </si>
+  <si>
+    <t>slideconfig errors</t>
+  </si>
+  <si>
+    <t>linechar</t>
+  </si>
+  <si>
+    <t>EBEGK31fas</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>1 = Huiswerk; 1 = Thuissituatie; 1 = Werk; 1 = Ouders</t>
+  </si>
+  <si>
+    <t>Percent</t>
+  </si>
+  <si>
+    <t>weegfactor2024; weegfactor2022; weegfactor2020; weegfactor2016</t>
+  </si>
+  <si>
+    <t>Heideveen</t>
+  </si>
+  <si>
+    <t>2; 1</t>
+  </si>
+  <si>
+    <t>slideconfig</t>
   </si>
 </sst>
 </file>
@@ -1054,10 +1372,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1357,9 +1671,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F0AA7A9-459B-4958-BBC2-94F84CFD8846}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1377,31 +1691,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1409,25 +1723,51 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>58</v>
+        <v>101</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>1</v>
+        <v>117</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1466,63 +1806,63 @@
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="G1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="P1" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>107</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="15"/>
@@ -1533,15 +1873,15 @@
         <v>1</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="15"/>
@@ -1552,15 +1892,15 @@
         <v>1</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="16"/>
@@ -1570,18 +1910,18 @@
         <v>1</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="9" t="s">
         <v>11</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>12</v>
       </c>
       <c r="D5" s="16">
         <v>1</v>
@@ -1592,498 +1932,498 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K5" s="2">
         <v>2024</v>
       </c>
       <c r="L5" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N5" s="2">
         <v>2</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>11</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>12</v>
       </c>
       <c r="D6" s="16">
         <v>0</v>
       </c>
       <c r="E6" s="10"/>
       <c r="J6" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K6" s="2">
         <v>2024</v>
       </c>
       <c r="L6" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N6" s="2">
         <v>2</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>16</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>17</v>
       </c>
       <c r="D7" s="16">
         <v>5</v>
       </c>
       <c r="E7" s="10"/>
       <c r="J7" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K7" s="2">
         <v>2024</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N7" s="2">
         <v>2</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="16">
         <v>1</v>
       </c>
       <c r="E8" s="10"/>
       <c r="J8" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K8" s="2">
         <v>2024</v>
       </c>
       <c r="L8" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N8" s="2">
         <v>2</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>51</v>
-      </c>
       <c r="E9" s="10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K9" s="2">
         <v>2024</v>
       </c>
       <c r="L9" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N9" s="2">
         <v>3</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E10" s="10"/>
       <c r="H10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K10" s="2">
         <v>2024</v>
       </c>
       <c r="L10" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N10" s="2">
         <v>3</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K11" s="2">
         <v>2024</v>
       </c>
       <c r="L11" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N11" s="2">
         <v>3</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K12" s="2">
         <v>2024</v>
       </c>
       <c r="L12" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N12" s="2">
         <v>3</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K13" s="2">
         <v>2024</v>
       </c>
       <c r="L13" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N13" s="2">
         <v>3</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="41.4" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="69" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E14" s="10"/>
       <c r="J14" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>63</v>
+        <v>104</v>
       </c>
       <c r="L14" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>65</v>
+        <v>106</v>
       </c>
       <c r="N14" s="2">
         <v>5</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="41.4" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="69" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>67</v>
-      </c>
       <c r="D15" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E15" s="10"/>
       <c r="J15" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>63</v>
+        <v>104</v>
       </c>
       <c r="L15" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>65</v>
+        <v>106</v>
       </c>
       <c r="N15" s="2">
         <v>5</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="69" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D16" s="16">
         <v>1</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K16" s="2">
         <v>2024</v>
       </c>
       <c r="L16" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N16" s="2">
         <v>6</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D17" s="16">
         <v>1</v>
       </c>
       <c r="E17" s="2"/>
       <c r="H17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I17" s="9"/>
       <c r="J17" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K17" s="2">
         <v>2024</v>
       </c>
       <c r="L17" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N17" s="2">
         <v>6</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18" s="16">
         <v>1</v>
       </c>
       <c r="E18" s="10"/>
       <c r="J18" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K18" s="2">
         <v>2024</v>
       </c>
       <c r="L18" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N18" s="2">
         <v>6</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D19" s="16">
         <v>1</v>
@@ -2092,231 +2432,243 @@
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
       <c r="J19" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="L19" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="N19" s="2">
         <v>6</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D20" s="16">
         <v>1</v>
       </c>
       <c r="E20" s="10"/>
       <c r="J20" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K20" s="2">
         <v>2024</v>
       </c>
       <c r="L20" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N20" s="2">
         <v>7</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E21" s="10"/>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
       <c r="J21" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K21" s="2">
         <v>2024</v>
       </c>
       <c r="L21" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N21" s="2">
         <v>7</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K22" s="2">
         <v>2024</v>
       </c>
       <c r="L22" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N22" s="2">
         <v>7</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K23" s="2">
         <v>2024</v>
       </c>
       <c r="L23" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N23" s="2">
         <v>7</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K24" s="2">
         <v>2024</v>
       </c>
       <c r="L24" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N24" s="2">
         <v>8</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:17" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K25" s="2">
         <v>2024</v>
       </c>
       <c r="L25" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N25" s="2">
         <v>8</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="L26" s="13"/>
+      <c r="N26" s="2">
+        <v>9</v>
+      </c>
+      <c r="O26" s="2" t="s">
+        <v>102</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:O21" xr:uid="{73A75041-D6C8-4C2F-941F-420EA079C5D1}"/>
@@ -2332,8 +2684,916 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="D217:D1048576" numberStoredAsText="1"/>
+    <ignoredError sqref="D216:D1048576" numberStoredAsText="1"/>
   </ignoredErrors>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D55FF392-33AC-4D08-BFDD-940CEAA7C405}">
+  <dimension ref="A1:Q26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="56.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" style="17" customWidth="1"/>
+    <col min="5" max="5" width="32.109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.44140625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="15.109375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.109375" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="8"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="2">
+        <v>1</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="8"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="2">
+        <v>1</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="10"/>
+      <c r="L4" s="13"/>
+      <c r="N4" s="2">
+        <v>1</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="16">
+        <v>1</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2">
+        <v>2024</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N5" s="2">
+        <v>2</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="16">
+        <v>0</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="J6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2">
+        <v>2024</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N6" s="2">
+        <v>2</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="16">
+        <v>5</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="J7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="2">
+        <v>2024</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N7" s="2">
+        <v>10</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="16">
+        <v>1</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="J8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" s="2">
+        <v>2024</v>
+      </c>
+      <c r="L8" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N8" s="2">
+        <v>2</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K9" s="2">
+        <v>2024</v>
+      </c>
+      <c r="L9" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N9" s="2">
+        <v>3</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="H10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K10" s="2">
+        <v>2024</v>
+      </c>
+      <c r="L10" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N10" s="2">
+        <v>3</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K11" s="2">
+        <v>2024</v>
+      </c>
+      <c r="L11" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N11" s="2">
+        <v>3</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" s="2">
+        <v>2024</v>
+      </c>
+      <c r="L12" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N12" s="2">
+        <v>3</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K13" s="2">
+        <v>2024</v>
+      </c>
+      <c r="L13" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N13" s="2">
+        <v>3</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="J14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="N14" s="2">
+        <v>5</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="69" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="J15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="L15" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="N15" s="2">
+        <v>5</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="69" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K16" s="2">
+        <v>2024</v>
+      </c>
+      <c r="L16" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N16" s="2">
+        <v>6</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="16">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="H17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" s="9"/>
+      <c r="J17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K17" s="2">
+        <v>2024</v>
+      </c>
+      <c r="L17" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N17" s="2">
+        <v>6</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D18" s="16">
+        <v>1</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="J18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K18" s="2">
+        <v>2024</v>
+      </c>
+      <c r="L18" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N18" s="2">
+        <v>6</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="16">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L19" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="N19" s="2">
+        <v>6</v>
+      </c>
+      <c r="O19" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="J20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K20" s="2">
+        <v>2024</v>
+      </c>
+      <c r="L20" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N20" s="2">
+        <v>7</v>
+      </c>
+      <c r="O20" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K21" s="2">
+        <v>2024</v>
+      </c>
+      <c r="L21" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N21" s="2">
+        <v>7</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K22" s="2">
+        <v>2024</v>
+      </c>
+      <c r="L22" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N22" s="2">
+        <v>7</v>
+      </c>
+      <c r="O22" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K23" s="2">
+        <v>2024</v>
+      </c>
+      <c r="L23" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N23" s="2">
+        <v>7</v>
+      </c>
+      <c r="O23" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K24" s="2">
+        <v>2024</v>
+      </c>
+      <c r="L24" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N24" s="2">
+        <v>8</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K25" s="2">
+        <v>2024</v>
+      </c>
+      <c r="L25" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N25" s="2">
+        <v>8</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="L26" s="13"/>
+      <c r="N26" s="2">
+        <v>9</v>
+      </c>
+      <c r="O26" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:O21" xr:uid="{73A75041-D6C8-4C2F-941F-420EA079C5D1}"/>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576" xr:uid="{055A60F5-9428-4308-BF54-AA9D88C6B397}">
+      <formula1>"none, dim, var"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J3" xr:uid="{153A5A6D-36FE-4671-B77E-A16E387B2973}">
+      <formula1>"basis, referentie, basis en referentie"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -2624,6 +3884,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -2637,15 +3906,6 @@
     </TaxKeywordTaxHTField>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2670,6 +3930,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0EF40A6-8528-4994-A94E-1AE934020AF5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFBB421F-7112-4B85-A662-9379706C03DC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2679,12 +3947,4 @@
     <ds:schemaRef ds:uri="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0EF40A6-8528-4994-A94E-1AE934020AF5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Nieuwe voorbeeld config toegevoegd
Hierin is de kolom CBS toegevoegd bij reports, zodat de CBS code van de betreffende gemeente ingelezen kan worden.
Ook is de time_val in gebruik voor het jaartal van de CBS data.
</commit_message>
<xml_diff>
--- a/example/config.xlsx
+++ b/example/config.xlsx
@@ -1,25 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanderve\OneDrive - VRLN\PSchijf\Gezondheidsmonitor\Algemeen\Automatisering en R\0. Github\report_excel_to_powerpoint\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stijn.michielse\Documents\reports_excel_to_powerpoint\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F360C7-580E-4BC7-811C-422536A8DCD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF16CF3D-75F7-471B-AA95-A327D2E0CD39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{340DDFAE-1A83-41FC-A379-531A17E4526A}"/>
+    <workbookView xWindow="930" yWindow="375" windowWidth="26880" windowHeight="13515" xr2:uid="{340DDFAE-1A83-41FC-A379-531A17E4526A}"/>
   </bookViews>
   <sheets>
     <sheet name="reports" sheetId="4" r:id="rId1"/>
     <sheet name="slideconfig" sheetId="6" r:id="rId2"/>
-    <sheet name="slideconfig errors" sheetId="7" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">slideconfig!$A$1:$O$21</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'slideconfig errors'!$A$1:$O$21</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -147,7 +145,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{32B406C9-7EFF-4D27-BDD2-3FA619BB13ED}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{32B406C9-7EFF-4D27-BDD2-3FA619BB13ED}">
       <text>
         <r>
           <rPr>
@@ -161,7 +159,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{A61A6616-02DD-4B95-AB2A-7FD23DC29B0C}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{A61A6616-02DD-4B95-AB2A-7FD23DC29B0C}">
       <text>
         <r>
           <rPr>
@@ -176,7 +174,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{7FF27BA5-84F4-4C4B-A70C-1F3AC0A67F25}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{7FF27BA5-84F4-4C4B-A70C-1F3AC0A67F25}">
       <text>
         <r>
           <rPr>
@@ -474,288 +472,8 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Vermeulen, Sander</author>
-  </authors>
-  <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{3A6DDAAC-DB96-4EDB-87F8-2D4C8310B620}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Deze kolom is multifunctioneel. Het gebruik van de kolom is afhankelijk van het type.
-Voor grafieken wordt deze kolom gebruikt als grafiektitel.
-Bij het type text_comparison wordt de tekst in deze kolom gebruikt om te bepalen welke vergelijking er moet worden gemaakt en welke vergelijkstext er moet worden gekozen afhankelijk van de uitkomst van de vergelijking.
-Bij het type percentage_in_text wordt deze kolom gebruikt om te bepalen waar de percentages moeten komen.
-Voor het type topN wordt deze kolom, naast de grafiektitel, ook gebruikt om te bepalen hoeveel variabelen moeten worden getoond.
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{841F10B0-B2BB-43CD-8ECC-BAA3558A5298}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Voer in deze kolom het type in dat moet worden gebruikt voor deze slideregel.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{A127A259-CF63-4784-87E7-B35CF39AA8B5}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Voer hier de variabelenaam of variabelenamen in waarvoor cijfers moeten worden berekend.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{A4C88C7D-40E4-47E4-94F6-8C62D181951E}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Voer hier de waarde in waarvoor cijfers moeten worden berekend. De waardes moeten overeenkomen met de opgegeven variabele naam in de kolom var. Als je meerdere variabelen hebt opgegeven in de kolom var dan geef je in deze kolom evenveel waardes op als variabelen. Scheid de waardes met een puntkomma ';'
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{D347B8B5-505A-46A1-93A7-402E51CAC44E}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>In deze kolom kun je per opgegeven waarde de waardelabels aanpassen. Stel je berekent het cijfer voor value 1 en het waarde label wil je veranderen naar 'Voelt zich gelukkig' dan doe je dat zo:
-1 = Voelt zich gelukkig
-Heb je meerdere variabelen opgegeven in de kolom var (en dus ook meerdere values in de kolom value) dan moet je aangepaste labels scheiden door een puntkomma ';'. Bijvoorbeeld:
-1 = Voelt zich gelukkig; 1 = Is weerbaar
-Het script gebruikt als deze kolom leeg is de labels die in dataset zitten. Je kunt de labels dus ook zelf aanpassen in de data.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{DB53629F-11D4-49B2-B8B2-029759700076}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Geef hier een variabele naam op als je de variabele(n) in de kolom var wilt berekenen voor verschillende groepen.
-Je kunt hier meerdere variabele namen opgegeven gescheiden door een puntkomma ';'. Als je dit doet worden voor elke variabele gegroepeerde cijfers berekend op de opgegeven variabelen in de kolom var. Wil je tegelijk groeperen op twee variabelen geef dan een van de variabelen op in grouping1 en de andere in grouping 2. Doe je dit binnen een staafgrafiek dan komt grouping1 op de x-as en grouping2 in de legenda.
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{24A47BC3-745F-472F-AC41-912F2B01801F}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Wil je de labels van de opgegeven variabele in kolom grouping1 aanpassen geef dat dan hier op.
-Voorbeeld:
-0 = M; 1 = J
-Let op dat dit niet kan als je meerdere variabelen opgeeft in de kolom grouping1 dat dit niet werkt. Het script gebruikt als deze kolom leeg is de labels die in dataset zitten. Je kunt de labels dus ook zelf aanpassen in de data.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{EBD45C9E-A560-44E4-94FA-F2D12EC76979}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Geef hier een variabele naam op als je de variabele(n) in de kolom var wilt berekenen voor verschillende groepen.
-Je kunt hier meerdere variabele namen opgegeven gescheiden door een puntkomma ';'. Als je dit doet worden voor elke variabele gegroepeerde cijfers berekend op de opgegeven variabelen in de kolom var. Wil je tegelijk groeperen op twee variabelen geef dan een van de variabelen op in grouping1 en de andere in grouping 2. Doe je dit binnen een staafgrafiek dan komt grouping1 op de x-as en grouping2 in de legenda.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{BCBAF521-D70C-4B7A-8C12-6182D13D42F9}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Wil je de labels van de opgegeven variabele in kolom grouping1 aanpassen geef dat dan hier op.
-Voorbeeld:
-0 = M; 1 = J
-Let op dat dit niet kan als je meerdere variabelen opgeeft in de kolom grouping1 dat dit niet werkt. Het script gebruikt als deze kolom leeg is de labels die in dataset zitten. Je kunt de labels dus ook zelf aanpassen in de data.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{FC4ADE40-53A6-45B3-B68F-A8871F0BC1B9}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Geef hier de variabele naam of namen op van de dimensies waarvoor cijfers moeten worden berekend. Deze variabele moet overeenkomen met een (of meer) van de variabelen die is opgegeven in de kolom dim_vars van de rapportconfiguratie (het eerste tabblad van dit Excel bestand).
-Geef je meerdere dimensie variabelen op scheid deze dan met een puntkomma ';'</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{2DE70DB4-0430-47E8-A03E-A8C4742E1601}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Vul hier de waarde in van de opgegeven time_var in de rapportconfiguratie waarvoor cijfers moeten worden berekend. Wil je voor meer dan een periode cijfersberekenen dan kun je meerdere waardes opgegeven gescheiden door een puntkomma ';'.
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{37CEB835-027D-4FDB-A33A-2C83A8C26F31}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Geef hier op wat voor type weging moet worden toegepast.
-Kies je voor 'none' dan worden ongewogen cijfers berekend.
-Kies je voor 'var' dan moet je per indicator een weegfactor variabele opgeven in de kolom weight_var.
-Kies je voor 'dim' dan wordt er gewogen op dimensieniveau. Hiervoor moet je de juiste weegfactor variabele(n) opgegeven in de rapportconfiguratie (eerste tabblad van dit Excel bestand).
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{821253B3-00D0-49D0-B44F-810F98C15DDB}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Als het weight_type var is en je dus weegt op variabele niveau dan geef je hier de weegfactor voor de variabele op. Varieert de weegfactor variabele afhankelijk van bijvoorbeeld het jaar dan kun je per opgegeven jaar in de time_val kolom een weegfactor opgeven gescheiden door een puntkomma ';'
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{B3C8EC77-516D-4853-91A8-238D004968BC}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Geef hier het slidenummer op waar de content geplaatst moet worden.
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{FBDED92D-F73E-4DC3-960B-85A3E379DAEF}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Geef hier de naam op van de tijdelijke aanduiding waar de content moet worden geplaatst op de opgegeven slide.
-Let op dat de opgegeven naam </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>exact</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> hetzelfde is.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{A1254F1B-23CD-424B-B31B-42CDBA4D1318}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Bij grafieken loopt de y-as standaard van 0 tot 1 (0 tot 100%). Om de hoogte van de y-as aan te passen kun je hier een waarde tussen 0 en 1 opgegeven.
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{37226A97-2FAE-439E-8294-18FA874A47D4}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">De standaard richting van alle staafgrafieken is verticaal. Wil je een horizontale staafgrafiek maken vul dan bij de desbetreffende regel horizontal in.
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="113">
   <si>
     <t>Zandwijk</t>
   </si>
@@ -1144,27 +862,6 @@
     <t>reportname</t>
   </si>
   <si>
-    <t>slideconfig errors</t>
-  </si>
-  <si>
-    <t>linechar</t>
-  </si>
-  <si>
-    <t>EBEGK31fas</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>1 = Huiswerk; 1 = Thuissituatie; 1 = Werk; 1 = Ouders</t>
-  </si>
-  <si>
-    <t>Percent</t>
-  </si>
-  <si>
-    <t>weegfactor2024; weegfactor2022; weegfactor2020; weegfactor2016</t>
-  </si>
-  <si>
     <t>Heideveen</t>
   </si>
   <si>
@@ -1172,6 +869,12 @@
   </si>
   <si>
     <t>slideconfig</t>
+  </si>
+  <si>
+    <t>GM0888</t>
+  </si>
+  <si>
+    <t>CBS</t>
   </si>
 </sst>
 </file>
@@ -1671,25 +1374,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F0AA7A9-459B-4958-BBC2-94F84CFD8846}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5546875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="20.21875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="23.44140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="20.44140625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="23.77734375" style="4" customWidth="1"/>
-    <col min="9" max="9" width="19.5546875" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="4"/>
+    <col min="2" max="2" width="27.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.42578125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="23.7109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="19.5703125" style="4" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>29</v>
       </c>
@@ -1709,16 +1414,19 @@
         <v>33</v>
       </c>
       <c r="G1" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1729,7 +1437,7 @@
         <v>56</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>48</v>
@@ -1737,16 +1445,19 @@
       <c r="F2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>101</v>
@@ -1755,18 +1466,21 @@
         <v>56</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>48</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="G3" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1782,29 +1496,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF87A273-214F-4086-84B2-968343C1FFDC}">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="56.33203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" style="17" customWidth="1"/>
-    <col min="5" max="5" width="32.109375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.44140625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="15.109375" style="3" customWidth="1"/>
-    <col min="14" max="14" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.109375" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="56.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="17" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.42578125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.140625" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>36</v>
       </c>
@@ -1857,7 +1573,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
@@ -1876,7 +1592,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
@@ -1895,7 +1611,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="51" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>69</v>
       </c>
@@ -1913,7 +1629,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>9</v>
       </c>
@@ -1950,7 +1666,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>13</v>
       </c>
@@ -1983,7 +1699,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>15</v>
       </c>
@@ -2016,7 +1732,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>18</v>
       </c>
@@ -2049,7 +1765,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>9</v>
       </c>
@@ -2087,7 +1803,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>9</v>
       </c>
@@ -2126,7 +1842,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>9</v>
       </c>
@@ -2162,7 +1878,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>9</v>
       </c>
@@ -2201,7 +1917,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>9</v>
       </c>
@@ -2240,7 +1956,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="69" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>18</v>
       </c>
@@ -2276,7 +1992,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="69" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>61</v>
       </c>
@@ -2309,7 +2025,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="69" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>73</v>
       </c>
@@ -2345,7 +2061,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>71</v>
       </c>
@@ -2382,7 +2098,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>74</v>
       </c>
@@ -2415,7 +2131,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>103</v>
       </c>
@@ -2450,7 +2166,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>81</v>
       </c>
@@ -2483,7 +2199,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>82</v>
       </c>
@@ -2518,7 +2234,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>83</v>
       </c>
@@ -2550,7 +2266,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>84</v>
       </c>
@@ -2582,7 +2298,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>98</v>
       </c>
@@ -2617,7 +2333,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>98</v>
       </c>
@@ -2655,12 +2371,15 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>99</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>100</v>
+      </c>
+      <c r="K26" s="2">
+        <v>2024</v>
       </c>
       <c r="L26" s="13"/>
       <c r="N26" s="2">
@@ -2690,915 +2409,32 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D55FF392-33AC-4D08-BFDD-940CEAA7C405}">
-  <dimension ref="A1:Q26"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="56.33203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" style="17" customWidth="1"/>
-    <col min="5" max="5" width="32.109375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.44140625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="15.109375" style="3" customWidth="1"/>
-    <col min="14" max="14" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.109375" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="8.88671875" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="M1" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="8"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="2">
-        <v>1</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="8"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="2">
-        <v>1</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="10"/>
-      <c r="L4" s="13"/>
-      <c r="N4" s="2">
-        <v>1</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="16">
-        <v>1</v>
-      </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K5" s="2">
-        <v>2024</v>
-      </c>
-      <c r="L5" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="N5" s="2">
-        <v>2</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="16">
-        <v>0</v>
-      </c>
-      <c r="E6" s="10"/>
-      <c r="J6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K6" s="2">
-        <v>2024</v>
-      </c>
-      <c r="L6" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="N6" s="2">
-        <v>2</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="16">
-        <v>5</v>
-      </c>
-      <c r="E7" s="10"/>
-      <c r="J7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K7" s="2">
-        <v>2024</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="N7" s="2">
-        <v>10</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="16">
-        <v>1</v>
-      </c>
-      <c r="E8" s="10"/>
-      <c r="J8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K8" s="2">
-        <v>2024</v>
-      </c>
-      <c r="L8" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="N8" s="2">
-        <v>2</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="K9" s="2">
-        <v>2024</v>
-      </c>
-      <c r="L9" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="N9" s="2">
-        <v>3</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="10"/>
-      <c r="H10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K10" s="2">
-        <v>2024</v>
-      </c>
-      <c r="L10" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="N10" s="2">
-        <v>3</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K11" s="2">
-        <v>2024</v>
-      </c>
-      <c r="L11" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="N11" s="2">
-        <v>3</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K12" s="2">
-        <v>2024</v>
-      </c>
-      <c r="L12" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="N12" s="2">
-        <v>3</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K13" s="2">
-        <v>2024</v>
-      </c>
-      <c r="L13" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="N13" s="2">
-        <v>3</v>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="10"/>
-      <c r="J14" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="L14" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="M14" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="N14" s="2">
-        <v>5</v>
-      </c>
-      <c r="O14" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="P14" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="69" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="10"/>
-      <c r="J15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="L15" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="N15" s="2">
-        <v>5</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="69" x14ac:dyDescent="0.3">
-      <c r="A16" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="16">
-        <v>1</v>
-      </c>
-      <c r="E16" s="10"/>
-      <c r="F16" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K16" s="2">
-        <v>2024</v>
-      </c>
-      <c r="L16" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="M16" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="N16" s="2">
-        <v>6</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="16">
-        <v>1</v>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="H17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I17" s="9"/>
-      <c r="J17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K17" s="2">
-        <v>2024</v>
-      </c>
-      <c r="L17" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="N17" s="2">
-        <v>6</v>
-      </c>
-      <c r="O17" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="D18" s="16">
-        <v>1</v>
-      </c>
-      <c r="E18" s="10"/>
-      <c r="J18" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="K18" s="2">
-        <v>2024</v>
-      </c>
-      <c r="L18" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="M18" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="N18" s="2">
-        <v>6</v>
-      </c>
-      <c r="O18" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="16">
-        <v>1</v>
-      </c>
-      <c r="E19" s="2"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="L19" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="M19" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="N19" s="2">
-        <v>6</v>
-      </c>
-      <c r="O19" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="E20" s="10"/>
-      <c r="J20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K20" s="2">
-        <v>2024</v>
-      </c>
-      <c r="L20" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="M20" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="N20" s="2">
-        <v>7</v>
-      </c>
-      <c r="O20" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E21" s="10"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="K21" s="2">
-        <v>2024</v>
-      </c>
-      <c r="L21" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="M21" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="N21" s="2">
-        <v>7</v>
-      </c>
-      <c r="O21" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K22" s="2">
-        <v>2024</v>
-      </c>
-      <c r="L22" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="M22" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="N22" s="2">
-        <v>7</v>
-      </c>
-      <c r="O22" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="K23" s="2">
-        <v>2024</v>
-      </c>
-      <c r="L23" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="M23" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="N23" s="2">
-        <v>7</v>
-      </c>
-      <c r="O23" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K24" s="2">
-        <v>2024</v>
-      </c>
-      <c r="L24" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="M24" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="N24" s="2">
-        <v>8</v>
-      </c>
-      <c r="O24" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K25" s="2">
-        <v>2024</v>
-      </c>
-      <c r="L25" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="M25" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="N25" s="2">
-        <v>8</v>
-      </c>
-      <c r="O25" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q25" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="L26" s="13"/>
-      <c r="N26" s="2">
-        <v>9</v>
-      </c>
-      <c r="O26" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:O21" xr:uid="{73A75041-D6C8-4C2F-941F-420EA079C5D1}"/>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576" xr:uid="{055A60F5-9428-4308-BF54-AA9D88C6B397}">
-      <formula1>"none, dim, var"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J3" xr:uid="{153A5A6D-36FE-4671-B77E-A16E387B2973}">
-      <formula1>"basis, referentie, basis en referentie"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4e95bed8-6d15-4403-ad70-a53422338dca">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94" xsi:nil="true"/>
+    <TaxKeywordTaxHTField xmlns="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C4EA295FB1FB9547A73C9F5819D6E613" ma:contentTypeVersion="22" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="c6ed9d5736a8b6bce7fdd25df6dc73c6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4e95bed8-6d15-4403-ad70-a53422338dca" xmlns:ns3="10d3344f-2d16-43d9-a145-97142f5cb288" xmlns:ns4="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9b8dd8ae3f6086a1cec4bb961aaa59ad" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3883,32 +2719,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0EF40A6-8528-4994-A94E-1AE934020AF5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4e95bed8-6d15-4403-ad70-a53422338dca">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94" xsi:nil="true"/>
-    <TaxKeywordTaxHTField xmlns="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFBB421F-7112-4B85-A662-9379706C03DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="4e95bed8-6d15-4403-ad70-a53422338dca"/>
+    <ds:schemaRef ds:uri="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{732D36F7-14D5-4012-B7CB-89E08DF70A9F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3927,24 +2758,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0EF40A6-8528-4994-A94E-1AE934020AF5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFBB421F-7112-4B85-A662-9379706C03DC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="4e95bed8-6d15-4403-ad70-a53422338dca"/>
-    <ds:schemaRef ds:uri="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Version 1.3 Patch Notes in README
</commit_message>
<xml_diff>
--- a/example/config.xlsx
+++ b/example/config.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vrln.sharepoint.com/sites/GGD-ONDZ/PSchijf/Gezondheidsmonitor/Algemeen/Automatisering en R/0. Github/report_excel_to_powerpoint/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{DF16CF3D-75F7-471B-AA95-A327D2E0CD39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D21D9A1-7A28-4A35-96D9-097FC98B3B30}"/>
+  <xr:revisionPtr revIDLastSave="318" documentId="13_ncr:1_{DF16CF3D-75F7-471B-AA95-A327D2E0CD39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40184E05-49A5-44EE-AF32-B5FFD2DA482D}"/>
   <bookViews>
-    <workbookView xWindow="-4695" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{340DDFAE-1A83-41FC-A379-531A17E4526A}"/>
+    <workbookView xWindow="3540" yWindow="17172" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{340DDFAE-1A83-41FC-A379-531A17E4526A}"/>
   </bookViews>
   <sheets>
     <sheet name="reports" sheetId="4" r:id="rId1"/>
     <sheet name="slideconfig" sheetId="6" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">slideconfig!$A$1:$O$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">slideconfig!$A$1:$O$38</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -188,7 +188,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{1BB86B92-42B5-47A4-8B4B-EC7CBF64DEB9}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{23C4A047-7C7A-401F-B1D8-552DC56BE473}">
       <text>
         <r>
           <rPr>
@@ -486,7 +486,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="151">
   <si>
     <t>Zandwijk</t>
   </si>
@@ -641,9 +641,6 @@
     <t>Zandwijk; Nederland</t>
   </si>
   <si>
-    <t>PBMHK3S3; EBEGK311</t>
-  </si>
-  <si>
     <t>dim_vars</t>
   </si>
   <si>
@@ -660,9 +657,6 @@
   </si>
   <si>
     <t>weegfactor2024</t>
-  </si>
-  <si>
-    <t>1 = Psychische klachten; 1 = Ervaren gezondheid</t>
   </si>
   <si>
     <t>linechart</t>
@@ -794,12 +788,6 @@
     <t>ylimit</t>
   </si>
   <si>
-    <t>0.3</t>
-  </si>
-  <si>
-    <t>0.5</t>
-  </si>
-  <si>
     <t>direction</t>
   </si>
   <si>
@@ -888,6 +876,134 @@
   </si>
   <si>
     <t>cbs_dim_code</t>
+  </si>
+  <si>
+    <t>Staafgrafiek 6</t>
+  </si>
+  <si>
+    <t>Staafgrafiek 7</t>
+  </si>
+  <si>
+    <t>Staafgrafiek 8</t>
+  </si>
+  <si>
+    <t>Staafgrafiek 9</t>
+  </si>
+  <si>
+    <t>Staafgrafiek 10</t>
+  </si>
+  <si>
+    <t>Staafgrafiek 11</t>
+  </si>
+  <si>
+    <t>GENDER; KLAS</t>
+  </si>
+  <si>
+    <t>PBMHK3S3; MCMZGB208; EBEGK311</t>
+  </si>
+  <si>
+    <t>1 = Heeft psychische klachten</t>
+  </si>
+  <si>
+    <t>Staafgrafiek 13</t>
+  </si>
+  <si>
+    <t>Staafgrafiek 14</t>
+  </si>
+  <si>
+    <t>Staafgrafiek 15</t>
+  </si>
+  <si>
+    <t>Staafgrafiek 17</t>
+  </si>
+  <si>
+    <t>Staafgrafiek 18</t>
+  </si>
+  <si>
+    <t>1; 2; 1</t>
+  </si>
+  <si>
+    <t>Variant 1</t>
+  </si>
+  <si>
+    <t>Variant 2</t>
+  </si>
+  <si>
+    <t>Variant 3</t>
+  </si>
+  <si>
+    <t>Variant 4</t>
+  </si>
+  <si>
+    <t>Variant 5</t>
+  </si>
+  <si>
+    <t>Variant 6</t>
+  </si>
+  <si>
+    <t>Variant 7</t>
+  </si>
+  <si>
+    <t>Variant 8</t>
+  </si>
+  <si>
+    <t>Variant 9</t>
+  </si>
+  <si>
+    <t>Variant 10</t>
+  </si>
+  <si>
+    <t>Variant 11</t>
+  </si>
+  <si>
+    <t>Variant 12</t>
+  </si>
+  <si>
+    <t>Variant 13</t>
+  </si>
+  <si>
+    <t>Variant 14</t>
+  </si>
+  <si>
+    <t>Variant 15</t>
+  </si>
+  <si>
+    <t>Variant 16</t>
+  </si>
+  <si>
+    <t>Variant 17</t>
+  </si>
+  <si>
+    <t>Variant 18</t>
+  </si>
+  <si>
+    <t>1 = Heeft psychische klachten; 2 = Geeft geen mantelzorg; 1 = Heeft een zeer goede gezondheid</t>
+  </si>
+  <si>
+    <t>1 = Heeft psychische klachten; 
+2 = Geeft geen mantelzorg; 
+1 = Heeft een zeer goede gezondheid</t>
+  </si>
+  <si>
+    <t>Staafgrafiek 12</t>
+  </si>
+  <si>
+    <t>Staafgrafiek 16</t>
+  </si>
+  <si>
+    <t>Staafgrafiek Variant 17 zonder aanpassingen</t>
+  </si>
+  <si>
+    <t>Staafgrafiek Variant 17 met aangepaste y-as</t>
+  </si>
+  <si>
+    <t>Staafgrafiek Variant 17 liggend</t>
+  </si>
+  <si>
+    <t>Staafgrafiek Variant 17 liggend met aangepaste y-as</t>
+  </si>
+  <si>
+    <t>0.5</t>
   </si>
 </sst>
 </file>
@@ -1088,10 +1204,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1393,24 +1505,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F0AA7A9-459B-4958-BBC2-94F84CFD8846}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5546875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="23.44140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="20.44140625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="23.6640625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="19.5546875" style="4" customWidth="1"/>
-    <col min="10" max="10" width="12.44140625" style="4" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="4"/>
+    <col min="2" max="2" width="27.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" style="4" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>29</v>
       </c>
@@ -1424,7 +1536,7 @@
         <v>35</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>33</v>
@@ -1439,21 +1551,21 @@
         <v>30</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>48</v>
@@ -1468,27 +1580,27 @@
         <v>2</v>
       </c>
       <c r="J2" s="16" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>48</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>50</v>
@@ -1497,7 +1609,7 @@
         <v>2</v>
       </c>
       <c r="J3" s="16" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1510,33 +1622,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF87A273-214F-4086-84B2-968343C1FFDC}">
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="56.33203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" style="17" customWidth="1"/>
-    <col min="5" max="5" width="32.109375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.44140625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="15.109375" style="3" customWidth="1"/>
-    <col min="14" max="14" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.109375" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="56.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="17" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.42578125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.140625" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>36</v>
       </c>
@@ -1550,19 +1660,19 @@
         <v>38</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>40</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>32</v>
@@ -1583,18 +1693,18 @@
         <v>44</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="15"/>
@@ -1608,7 +1718,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
@@ -1627,9 +1737,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="51" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>46</v>
@@ -1645,7 +1755,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>9</v>
       </c>
@@ -1673,7 +1783,7 @@
         <v>37</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N5" s="2">
         <v>2</v>
@@ -1682,7 +1792,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>13</v>
       </c>
@@ -1706,7 +1816,7 @@
         <v>37</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N6" s="2">
         <v>2</v>
@@ -1715,7 +1825,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>15</v>
       </c>
@@ -1739,7 +1849,7 @@
         <v>37</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N7" s="2">
         <v>2</v>
@@ -1748,7 +1858,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>18</v>
       </c>
@@ -1772,7 +1882,7 @@
         <v>37</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N8" s="2">
         <v>2</v>
@@ -1781,24 +1891,24 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>9</v>
+        <v>124</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="K9" s="2">
         <v>2024</v>
@@ -1807,7 +1917,7 @@
         <v>37</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N9" s="2">
         <v>3</v>
@@ -1815,26 +1925,22 @@
       <c r="O9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="P9" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>9</v>
+        <v>125</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>11</v>
+        <v>116</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="10"/>
-      <c r="H10" s="2" t="s">
-        <v>22</v>
+        <v>123</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>143</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>1</v>
@@ -1846,7 +1952,7 @@
         <v>37</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N10" s="2">
         <v>3</v>
@@ -1854,13 +1960,10 @@
       <c r="O10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Q10" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>9</v>
+        <v>126</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>47</v>
@@ -1871,12 +1974,11 @@
       <c r="D11" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="2" t="s">
-        <v>24</v>
+      <c r="E11" s="10" t="s">
+        <v>117</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="K11" s="2">
         <v>2024</v>
@@ -1885,7 +1987,7 @@
         <v>37</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N11" s="2">
         <v>3</v>
@@ -1894,28 +1996,24 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>9</v>
+        <v>127</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>11</v>
+        <v>116</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>22</v>
+        <v>123</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>142</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="K12" s="2">
         <v>2024</v>
@@ -1924,7 +2022,7 @@
         <v>37</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N12" s="2">
         <v>3</v>
@@ -1933,9 +2031,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>9</v>
+        <v>128</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>47</v>
@@ -1946,9 +2044,11 @@
       <c r="D13" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="2"/>
+      <c r="E13" s="10" t="s">
+        <v>117</v>
+      </c>
       <c r="F13" s="2" t="s">
-        <v>72</v>
+        <v>22</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>1</v>
@@ -1960,103 +2060,109 @@
         <v>37</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N13" s="2">
         <v>3</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="69" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>18</v>
+        <v>129</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>16</v>
+        <v>116</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="10"/>
+        <v>123</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="J14" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>104</v>
+        <v>1</v>
+      </c>
+      <c r="K14" s="2">
+        <v>2024</v>
       </c>
       <c r="L14" s="13" t="s">
         <v>37</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>106</v>
+        <v>56</v>
       </c>
       <c r="N14" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="P14" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="69" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>61</v>
+        <v>130</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="D15" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="10"/>
+      <c r="E15" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="J15" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K15" s="2" t="s">
-        <v>104</v>
+      <c r="K15" s="2">
+        <v>2024</v>
       </c>
       <c r="L15" s="13" t="s">
         <v>37</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>106</v>
+        <v>56</v>
       </c>
       <c r="N15" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="69" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>73</v>
+        <v>131</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="16">
-        <v>1</v>
-      </c>
-      <c r="E16" s="10"/>
-      <c r="F16" s="2" t="s">
-        <v>72</v>
+        <v>116</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>1</v>
@@ -2068,35 +2174,36 @@
         <v>37</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N16" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="41.4" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>71</v>
+        <v>132</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="16">
-        <v>1</v>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="H17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I17" s="9"/>
+        <v>11</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="J17" s="2" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="K17" s="2">
         <v>2024</v>
@@ -2105,29 +2212,34 @@
         <v>37</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N17" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>74</v>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>133</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="16">
-        <v>1</v>
-      </c>
-      <c r="E18" s="10"/>
+        <v>116</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="J18" s="2" t="s">
         <v>48</v>
       </c>
@@ -2138,64 +2250,72 @@
         <v>37</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N18" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>103</v>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>134</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="16">
-        <v>1</v>
-      </c>
-      <c r="E19" s="2"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
+        <v>11</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="J19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>105</v>
+        <v>48</v>
+      </c>
+      <c r="K19" s="2">
+        <v>2024</v>
       </c>
       <c r="L19" s="13" t="s">
         <v>37</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="N19" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
-        <v>81</v>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>135</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="16">
-        <v>1</v>
-      </c>
-      <c r="E20" s="10"/>
+        <v>11</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>115</v>
+      </c>
       <c r="J20" s="2" t="s">
         <v>1</v>
       </c>
@@ -2206,33 +2326,36 @@
         <v>37</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N20" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="12" t="s">
-        <v>82</v>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>136</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>16</v>
+        <v>116</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E21" s="10"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
+        <v>123</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>115</v>
+      </c>
       <c r="J21" s="2" t="s">
-        <v>85</v>
+        <v>1</v>
       </c>
       <c r="K21" s="2">
         <v>2024</v>
@@ -2241,27 +2364,33 @@
         <v>37</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N21" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="12" t="s">
-        <v>83</v>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>137</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>80</v>
+        <v>11</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>49</v>
+        <v>21</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>1</v>
@@ -2273,30 +2402,39 @@
         <v>37</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N22" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="12" t="s">
-        <v>84</v>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>138</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>80</v>
+        <v>11</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>49</v>
+        <v>21</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>85</v>
+        <v>1</v>
       </c>
       <c r="K23" s="2">
         <v>2024</v>
@@ -2305,30 +2443,36 @@
         <v>37</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N23" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="69" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>98</v>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>139</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>96</v>
+        <v>47</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>1</v>
@@ -2340,33 +2484,36 @@
         <v>37</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N24" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" ht="69" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>98</v>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>140</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>96</v>
+        <v>47</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="K25" s="2">
         <v>2024</v>
@@ -2375,38 +2522,649 @@
         <v>37</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N25" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q25" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>99</v>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>141</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>100</v>
+        <v>47</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="K26" s="2">
         <v>2024</v>
       </c>
-      <c r="L26" s="13"/>
+      <c r="L26" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="N26" s="2">
+        <v>6</v>
+      </c>
+      <c r="O26" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K27" s="2">
+        <v>2024</v>
+      </c>
+      <c r="L27" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N27" s="2">
+        <v>7</v>
+      </c>
+      <c r="O27" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K28" s="2">
+        <v>2024</v>
+      </c>
+      <c r="L28" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M28" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N28" s="2">
+        <v>7</v>
+      </c>
+      <c r="O28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K29" s="2">
+        <v>2024</v>
+      </c>
+      <c r="L29" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N29" s="2">
+        <v>7</v>
+      </c>
+      <c r="O29" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q29" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K30" s="2">
+        <v>2024</v>
+      </c>
+      <c r="L30" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N30" s="2">
+        <v>7</v>
+      </c>
+      <c r="O30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P30" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q30" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="10"/>
+      <c r="J31" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="L31" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M31" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="N31" s="2">
+        <v>8</v>
+      </c>
+      <c r="O31" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" s="10"/>
+      <c r="J32" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="L32" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M32" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="N32" s="2">
+        <v>8</v>
+      </c>
+      <c r="O32" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="16">
+        <v>1</v>
+      </c>
+      <c r="E33" s="10"/>
+      <c r="F33" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K33" s="2">
+        <v>2024</v>
+      </c>
+      <c r="L33" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M33" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N33" s="2">
         <v>9</v>
       </c>
-      <c r="O26" s="2" t="s">
-        <v>102</v>
+      <c r="O33" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" s="16">
+        <v>1</v>
+      </c>
+      <c r="E34" s="2"/>
+      <c r="H34" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I34" s="9"/>
+      <c r="J34" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K34" s="2">
+        <v>2024</v>
+      </c>
+      <c r="L34" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M34" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N34" s="2">
+        <v>9</v>
+      </c>
+      <c r="O34" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="16">
+        <v>1</v>
+      </c>
+      <c r="E35" s="10"/>
+      <c r="J35" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K35" s="2">
+        <v>2024</v>
+      </c>
+      <c r="L35" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M35" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N35" s="2">
+        <v>9</v>
+      </c>
+      <c r="O35" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" s="16">
+        <v>1</v>
+      </c>
+      <c r="E36" s="2"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="L36" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M36" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="N36" s="2">
+        <v>9</v>
+      </c>
+      <c r="O36" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" s="16">
+        <v>1</v>
+      </c>
+      <c r="E37" s="10"/>
+      <c r="J37" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K37" s="2">
+        <v>2024</v>
+      </c>
+      <c r="L37" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M37" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N37" s="2">
+        <v>10</v>
+      </c>
+      <c r="O37" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E38" s="10"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K38" s="2">
+        <v>2024</v>
+      </c>
+      <c r="L38" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M38" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N38" s="2">
+        <v>10</v>
+      </c>
+      <c r="O38" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A39" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K39" s="2">
+        <v>2024</v>
+      </c>
+      <c r="L39" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M39" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N39" s="2">
+        <v>10</v>
+      </c>
+      <c r="O39" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K40" s="2">
+        <v>2024</v>
+      </c>
+      <c r="L40" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M40" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N40" s="2">
+        <v>10</v>
+      </c>
+      <c r="O40" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K41" s="2">
+        <v>2024</v>
+      </c>
+      <c r="L41" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M41" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N41" s="2">
+        <v>11</v>
+      </c>
+      <c r="O41" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K42" s="2">
+        <v>2024</v>
+      </c>
+      <c r="L42" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M42" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N42" s="2">
+        <v>11</v>
+      </c>
+      <c r="O42" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q42" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K43" s="2">
+        <v>2024</v>
+      </c>
+      <c r="L43" s="13"/>
+      <c r="N43" s="2">
+        <v>12</v>
+      </c>
+      <c r="O43" s="2" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O21" xr:uid="{73A75041-D6C8-4C2F-941F-420EA079C5D1}"/>
+  <autoFilter ref="A1:O38" xr:uid="{73A75041-D6C8-4C2F-941F-420EA079C5D1}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J3" xr:uid="{F37CAFEA-4CF5-4746-8B55-2193B50B102D}">
@@ -2419,38 +3177,13 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="D216:D1048576" numberStoredAsText="1"/>
+    <ignoredError sqref="D233:D1048576" numberStoredAsText="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4e95bed8-6d15-4403-ad70-a53422338dca">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94" xsi:nil="true"/>
-    <TaxKeywordTaxHTField xmlns="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C4EA295FB1FB9547A73C9F5819D6E613" ma:contentTypeVersion="22" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="c6ed9d5736a8b6bce7fdd25df6dc73c6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4e95bed8-6d15-4403-ad70-a53422338dca" xmlns:ns3="10d3344f-2d16-43d9-a145-97142f5cb288" xmlns:ns4="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9b8dd8ae3f6086a1cec4bb961aaa59ad" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2735,27 +3468,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0EF40A6-8528-4994-A94E-1AE934020AF5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4e95bed8-6d15-4403-ad70-a53422338dca">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94" xsi:nil="true"/>
+    <TaxKeywordTaxHTField xmlns="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFBB421F-7112-4B85-A662-9379706C03DC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="4e95bed8-6d15-4403-ad70-a53422338dca"/>
-    <ds:schemaRef ds:uri="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{732D36F7-14D5-4012-B7CB-89E08DF70A9F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2774,4 +3512,24 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFBB421F-7112-4B85-A662-9379706C03DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="4e95bed8-6d15-4403-ad70-a53422338dca"/>
+    <ds:schemaRef ds:uri="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0EF40A6-8528-4994-A94E-1AE934020AF5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Version 1.3.1 Patch Notes in README
</commit_message>
<xml_diff>
--- a/example/config.xlsx
+++ b/example/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vrln.sharepoint.com/sites/GGD-ONDZ/PSchijf/Gezondheidsmonitor/Algemeen/Automatisering en R/0. Github/report_excel_to_powerpoint/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="318" documentId="13_ncr:1_{DF16CF3D-75F7-471B-AA95-A327D2E0CD39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40184E05-49A5-44EE-AF32-B5FFD2DA482D}"/>
+  <xr:revisionPtr revIDLastSave="319" documentId="13_ncr:1_{DF16CF3D-75F7-471B-AA95-A327D2E0CD39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F2A51CD-7EBE-4085-9F17-28CC777337C5}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="17172" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{340DDFAE-1A83-41FC-A379-531A17E4526A}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{340DDFAE-1A83-41FC-A379-531A17E4526A}"/>
   </bookViews>
   <sheets>
     <sheet name="reports" sheetId="4" r:id="rId1"/>
@@ -1624,7 +1624,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF87A273-214F-4086-84B2-968343C1FFDC}">
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3184,6 +3187,31 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4e95bed8-6d15-4403-ad70-a53422338dca">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94" xsi:nil="true"/>
+    <TaxKeywordTaxHTField xmlns="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C4EA295FB1FB9547A73C9F5819D6E613" ma:contentTypeVersion="22" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="c6ed9d5736a8b6bce7fdd25df6dc73c6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4e95bed8-6d15-4403-ad70-a53422338dca" xmlns:ns3="10d3344f-2d16-43d9-a145-97142f5cb288" xmlns:ns4="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9b8dd8ae3f6086a1cec4bb961aaa59ad" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3468,32 +3496,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4e95bed8-6d15-4403-ad70-a53422338dca">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94" xsi:nil="true"/>
-    <TaxKeywordTaxHTField xmlns="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFBB421F-7112-4B85-A662-9379706C03DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="4e95bed8-6d15-4403-ad70-a53422338dca"/>
+    <ds:schemaRef ds:uri="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0EF40A6-8528-4994-A94E-1AE934020AF5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{732D36F7-14D5-4012-B7CB-89E08DF70A9F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3512,24 +3535,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFBB421F-7112-4B85-A662-9379706C03DC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="4e95bed8-6d15-4403-ad70-a53422338dca"/>
-    <ds:schemaRef ds:uri="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0EF40A6-8528-4994-A94E-1AE934020AF5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Version 1.3.2 Patch Notes in README
</commit_message>
<xml_diff>
--- a/example/config.xlsx
+++ b/example/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vrln.sharepoint.com/sites/GGD-ONDZ/PSchijf/Gezondheidsmonitor/Algemeen/Automatisering en R/0. Github/report_excel_to_powerpoint/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="319" documentId="13_ncr:1_{DF16CF3D-75F7-471B-AA95-A327D2E0CD39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F2A51CD-7EBE-4085-9F17-28CC777337C5}"/>
+  <xr:revisionPtr revIDLastSave="347" documentId="13_ncr:1_{DF16CF3D-75F7-471B-AA95-A327D2E0CD39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57596CE9-2841-4DD3-B4EE-90DEAB0D94C3}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{340DDFAE-1A83-41FC-A379-531A17E4526A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{340DDFAE-1A83-41FC-A379-531A17E4526A}"/>
   </bookViews>
   <sheets>
     <sheet name="reports" sheetId="4" r:id="rId1"/>
@@ -295,7 +295,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Geef hier een variabele naam op als je de variabele(n) in de kolom var wilt berekenen voor verschillende groepen.
+          <t xml:space="preserve">Geef hier een variabele naam op als je de cijfers voor de variabele(n) in de kolom var wilt berekenen voor verschillende groepen.
 Je kunt hier meerdere variabele namen opgegeven gescheiden door een puntkomma ';'. Als je dit doet worden voor elke variabele gegroepeerde cijfers berekend op de opgegeven variabelen in de kolom var. Wil je tegelijk groeperen op twee variabelen geef dan een van de variabelen op in grouping1 en de andere in grouping 2. Doe je dit binnen een staafgrafiek dan komt grouping1 op de x-as en grouping2 in de legenda.
 </t>
         </r>
@@ -326,7 +326,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Geef hier een variabele naam op als je de variabele(n) in de kolom var wilt berekenen voor verschillende groepen.
+          <t>Geef hier een variabele naam op als je de cijfers voor de variabele(n) in de kolom var wilt berekenen voor verschillende groepen.
 Je kunt hier meerdere variabele namen opgegeven gescheiden door een puntkomma ';'. Als je dit doet worden voor elke variabele gegroepeerde cijfers berekend op de opgegeven variabelen in de kolom var. Wil je tegelijk groeperen op twee variabelen geef dan een van de variabelen op in grouping1 en de andere in grouping 2. Doe je dit binnen een staafgrafiek dan komt grouping1 op de x-as en grouping2 in de legenda.</t>
         </r>
       </text>
@@ -481,12 +481,33 @@
         </r>
       </text>
     </comment>
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{61A488C8-C1DB-4B48-AEC5-482C8110D90C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Bepaal hier de positie van de legenda.
+Als je deze kolom leegt laat wordt de default waarde b (bottom) gebruikt.
+b = onderaan (bottom)
+tr = rechtsboven (top right)
+l = links (left)
+r = rechts (right)
+t = bovenaan (top)
+n = geen legenda (none)
+Deze instelling werkt niet voor het type linechart. Wil je de legendapositie van type_linechart() aanpassen dan moet je de functie bewerken in type_linechart.R. Deze staat standaard op "bottom". Zoek binnen de functie op "bottom" en vervang dit door "none", "left", "right", "top" of "inside".</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="154">
   <si>
     <t>Zandwijk</t>
   </si>
@@ -1005,6 +1026,15 @@
   <si>
     <t>0.5</t>
   </si>
+  <si>
+    <t>legend_position</t>
+  </si>
+  <si>
+    <t>GENDER; KLAS; MBOKK3S32</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
 </sst>
 </file>
 
@@ -1013,7 +1043,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1098,6 +1128,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1622,11 +1658,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF87A273-214F-4086-84B2-968343C1FFDC}">
-  <dimension ref="A1:Q43"/>
+  <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1646,10 +1682,12 @@
     <col min="13" max="13" width="15.140625" style="3" customWidth="1"/>
     <col min="14" max="14" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.140625" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="8.85546875" style="2"/>
+    <col min="16" max="17" width="8.85546875" style="2"/>
+    <col min="18" max="18" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>36</v>
       </c>
@@ -1701,8 +1739,11 @@
       <c r="Q1" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R1" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
@@ -1721,7 +1762,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
@@ -1740,7 +1781,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="51" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="51" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>67</v>
       </c>
@@ -1758,7 +1799,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>9</v>
       </c>
@@ -1795,7 +1836,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>13</v>
       </c>
@@ -1828,7 +1869,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>15</v>
       </c>
@@ -1861,7 +1902,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>18</v>
       </c>
@@ -1894,7 +1935,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>124</v>
       </c>
@@ -1929,7 +1970,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>125</v>
       </c>
@@ -1964,7 +2005,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>126</v>
       </c>
@@ -1999,7 +2040,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>127</v>
       </c>
@@ -2034,7 +2075,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>128</v>
       </c>
@@ -2072,7 +2113,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>129</v>
       </c>
@@ -2110,7 +2151,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>130</v>
       </c>
@@ -2148,7 +2189,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>131</v>
       </c>
@@ -2186,7 +2227,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>132</v>
       </c>
@@ -2224,7 +2265,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>133</v>
       </c>
@@ -2262,7 +2303,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>134</v>
       </c>
@@ -2300,7 +2341,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>135</v>
       </c>
@@ -2316,8 +2357,8 @@
       <c r="E20" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>115</v>
+      <c r="F20" s="3" t="s">
+        <v>152</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>1</v>
@@ -2337,8 +2378,14 @@
       <c r="O20" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="Q20" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>136</v>
       </c>
@@ -2376,7 +2423,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>137</v>
       </c>
@@ -2414,7 +2461,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>138</v>
       </c>
@@ -2455,7 +2502,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>139</v>
       </c>
@@ -2496,7 +2543,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>140</v>
       </c>
@@ -2534,7 +2581,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>141</v>
       </c>
@@ -2572,7 +2619,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>146</v>
       </c>
@@ -2610,7 +2657,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>147</v>
       </c>
@@ -2651,7 +2698,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>148</v>
       </c>
@@ -2692,7 +2739,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>149</v>
       </c>
@@ -2736,7 +2783,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>18</v>
       </c>
@@ -2769,7 +2816,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>59</v>
       </c>
@@ -3187,22 +3234,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4e95bed8-6d15-4403-ad70-a53422338dca">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94" xsi:nil="true"/>
-    <TaxKeywordTaxHTField xmlns="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -3211,7 +3242,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C4EA295FB1FB9547A73C9F5819D6E613" ma:contentTypeVersion="22" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="c6ed9d5736a8b6bce7fdd25df6dc73c6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4e95bed8-6d15-4403-ad70-a53422338dca" xmlns:ns3="10d3344f-2d16-43d9-a145-97142f5cb288" xmlns:ns4="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9b8dd8ae3f6086a1cec4bb961aaa59ad" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3496,19 +3527,23 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFBB421F-7112-4B85-A662-9379706C03DC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="4e95bed8-6d15-4403-ad70-a53422338dca"/>
-    <ds:schemaRef ds:uri="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4e95bed8-6d15-4403-ad70-a53422338dca">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94" xsi:nil="true"/>
+    <TaxKeywordTaxHTField xmlns="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0EF40A6-8528-4994-A94E-1AE934020AF5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -3516,7 +3551,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{732D36F7-14D5-4012-B7CB-89E08DF70A9F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3535,4 +3570,16 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFBB421F-7112-4B85-A662-9379706C03DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="4e95bed8-6d15-4403-ad70-a53422338dca"/>
+    <ds:schemaRef ds:uri="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>